<commit_message>
Integrate Agora data for land/FoFObE and land/ICoLUPpUA
</commit_message>
<xml_diff>
--- a/InputData/land/FoFObE/Fraction of Forests Owned by Entity.xlsx
+++ b/InputData/land/FoFObE/Fraction of Forests Owned by Entity.xlsx
@@ -1,27 +1,39 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23328"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Meghan\Dropbox (Energy Innovation)\EPS Versions\eps-1.5.0-us-wipL\InputData\land\FoFObE\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mdeng\Dropbox (Energy Innovation)\EU EPS\InputData\land\FoFObE\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{978EB6DA-0A4F-474B-A4E4-4017324A82D5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="90" windowWidth="19140" windowHeight="9270"/>
+    <workbookView xWindow="40275" yWindow="4980" windowWidth="20625" windowHeight="14865" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
     <sheet name="Data" sheetId="2" r:id="rId2"/>
     <sheet name="FoFObE" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
   <si>
     <t>FoFObE Fraction of Forests Owned by Entity</t>
   </si>
@@ -29,63 +41,12 @@
     <t>Source:</t>
   </si>
   <si>
-    <t>National Forest</t>
-  </si>
-  <si>
-    <t>Other public</t>
-  </si>
-  <si>
-    <t>Forest industry</t>
-  </si>
-  <si>
-    <t>Other private</t>
-  </si>
-  <si>
-    <t>Timber land</t>
-  </si>
-  <si>
-    <t>Reserved forest</t>
-  </si>
-  <si>
-    <t>Other forest</t>
-  </si>
-  <si>
-    <t>U.S.</t>
-  </si>
-  <si>
-    <t>Ownership of Forest Land (million hectares)</t>
-  </si>
-  <si>
-    <t>U.S. Forest Service</t>
-  </si>
-  <si>
-    <t>U.S. Forest Facts and Historical Trends</t>
-  </si>
-  <si>
-    <t>http://www.fia.fs.fed.us/library/briefings-summaries-overviews/docs/ForestFactsMetric.pdf</t>
-  </si>
-  <si>
-    <t>Page 6</t>
-  </si>
-  <si>
     <t>government</t>
   </si>
   <si>
     <t>Notes</t>
   </si>
   <si>
-    <t>The amount of government-owned forest is provided in the table.</t>
-  </si>
-  <si>
-    <t>We assume that all privately-owned forest used for timber land is owned</t>
-  </si>
-  <si>
-    <t>by industry, and half of the remaining privately-owned forest land is owned</t>
-  </si>
-  <si>
-    <t>by industry.  The remainder is owned by consumers.</t>
-  </si>
-  <si>
     <t>foreign entities</t>
   </si>
   <si>
@@ -135,12 +96,51 @@
   </si>
   <si>
     <t>Fraction of Forest Owned (dimensionless)</t>
+  </si>
+  <si>
+    <t>http://www.unece.org/fileadmin/DAM/timber/publications/SP-26.pdf</t>
+  </si>
+  <si>
+    <t>Page 5, paragraph 3</t>
+  </si>
+  <si>
+    <t>Page 10, paragraph 1</t>
+  </si>
+  <si>
+    <t>We assume that these holdings belong to private individuals</t>
+  </si>
+  <si>
+    <t>On page 5, the share of privately owned forests is documented.</t>
+  </si>
+  <si>
+    <t>On page 10, we find the share of holdings smaller than 5 ha.</t>
+  </si>
+  <si>
+    <t>while the rest is owned by corporations.</t>
+  </si>
+  <si>
+    <t>Share of publicly owned forests</t>
+  </si>
+  <si>
+    <t>Share of privately owned forests</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Share of holdings larger than 5 ha </t>
+  </si>
+  <si>
+    <t>United Nations</t>
+  </si>
+  <si>
+    <t>Geneva Timber and Forest Study Paper 26: Private Forest Ownership in Europe</t>
+  </si>
+  <si>
+    <t>Share of private holdings smaller than 5 ha</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
@@ -190,20 +190,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
@@ -301,6 +295,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -336,6 +347,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -511,12 +539,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
@@ -528,251 +556,668 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>11</v>
+        <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="B4" s="3">
-        <v>2001</v>
+      <c r="B4" s="2">
+        <v>2010</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B5" t="s">
-        <v>12</v>
+        <v>32</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="B6" s="4" t="s">
-        <v>13</v>
+      <c r="B6" s="3" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B7" t="s">
-        <v>14</v>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="B8" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A9" s="1" t="s">
-        <v>16</v>
+        <v>3</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A15" s="1" t="s">
-        <v>36</v>
+        <v>19</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
-        <v>29</v>
+        <v>12</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
-        <v>30</v>
+        <v>13</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
-        <v>31</v>
+        <v>14</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
-        <v>32</v>
+        <v>15</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
-        <v>33</v>
+        <v>16</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
-        <v>34</v>
+        <v>17</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
-        <v>35</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="B6" r:id="rId1"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId2"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B18"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A2:N35"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="17.3984375" customWidth="1"/>
+    <col min="1" max="1" width="32.86328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="B2" s="6" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A3" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="1">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A4" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A5" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A6" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B6">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A7" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B7" s="1">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A8" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B8">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A9" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B9">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A10" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B10">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A11" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B11" s="1">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A12" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B12">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A13" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A14" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A15" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B15" s="1">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A16" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B16">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A17" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A18" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B18">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="A2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B2" s="4">
+        <v>0.501</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="A3" s="4" t="s">
         <v>29</v>
       </c>
+      <c r="B3" s="4">
+        <f>1-B2</f>
+        <v>0.499</v>
+      </c>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
+      <c r="G3" s="4"/>
+      <c r="H3" s="4"/>
+      <c r="I3" s="4"/>
+      <c r="J3" s="4"/>
+      <c r="K3" s="4"/>
+      <c r="L3" s="4"/>
+      <c r="M3" s="4"/>
+      <c r="N3" s="4"/>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="A4" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B4" s="4">
+        <f>0.86*B3</f>
+        <v>0.42913999999999997</v>
+      </c>
+      <c r="C4" s="4"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4"/>
+      <c r="G4" s="4"/>
+      <c r="H4" s="4"/>
+      <c r="I4" s="4"/>
+      <c r="J4" s="4"/>
+      <c r="K4" s="4"/>
+      <c r="L4" s="4"/>
+      <c r="M4" s="4"/>
+      <c r="N4" s="4"/>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="A5" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B5" s="4">
+        <f>B3-B4</f>
+        <v>6.9860000000000033E-2</v>
+      </c>
+      <c r="C5" s="4"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="4"/>
+      <c r="F5" s="4"/>
+      <c r="G5" s="4"/>
+      <c r="H5" s="4"/>
+      <c r="I5" s="4"/>
+      <c r="J5" s="4"/>
+      <c r="K5" s="4"/>
+      <c r="L5" s="4"/>
+      <c r="M5" s="4"/>
+      <c r="N5" s="4"/>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="A6" s="4"/>
+      <c r="B6" s="4"/>
+      <c r="C6" s="4"/>
+      <c r="D6" s="4"/>
+      <c r="E6" s="4"/>
+      <c r="F6" s="4"/>
+      <c r="G6" s="4"/>
+      <c r="H6" s="4"/>
+      <c r="I6" s="4"/>
+      <c r="J6" s="4"/>
+      <c r="K6" s="4"/>
+      <c r="L6" s="4"/>
+      <c r="M6" s="4"/>
+      <c r="N6" s="4"/>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="A7" s="4"/>
+      <c r="B7" s="4"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="4"/>
+      <c r="G7" s="4"/>
+      <c r="H7" s="4"/>
+      <c r="I7" s="4"/>
+      <c r="J7" s="4"/>
+      <c r="K7" s="4"/>
+      <c r="L7" s="4"/>
+      <c r="M7" s="4"/>
+      <c r="N7" s="4"/>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="A8" s="4"/>
+      <c r="B8" s="4"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4"/>
+      <c r="F8" s="4"/>
+      <c r="G8" s="4"/>
+      <c r="H8" s="4"/>
+      <c r="I8" s="4"/>
+      <c r="J8" s="4"/>
+      <c r="K8" s="4"/>
+      <c r="L8" s="4"/>
+      <c r="M8" s="4"/>
+      <c r="N8" s="4"/>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="A9" s="4"/>
+      <c r="B9" s="4"/>
+      <c r="C9" s="4"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="4"/>
+      <c r="F9" s="4"/>
+      <c r="G9" s="4"/>
+      <c r="H9" s="4"/>
+      <c r="I9" s="4"/>
+      <c r="J9" s="4"/>
+      <c r="K9" s="4"/>
+      <c r="L9" s="4"/>
+      <c r="M9" s="4"/>
+      <c r="N9" s="4"/>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="A10" s="4"/>
+      <c r="B10" s="4"/>
+      <c r="C10" s="4"/>
+      <c r="D10" s="4"/>
+      <c r="E10" s="4"/>
+      <c r="F10" s="4"/>
+      <c r="G10" s="4"/>
+      <c r="H10" s="4"/>
+      <c r="I10" s="4"/>
+      <c r="J10" s="4"/>
+      <c r="K10" s="4"/>
+      <c r="L10" s="4"/>
+      <c r="M10" s="4"/>
+      <c r="N10" s="4"/>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="A11" s="4"/>
+      <c r="B11" s="4"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="4"/>
+      <c r="E11" s="4"/>
+      <c r="F11" s="4"/>
+      <c r="G11" s="4"/>
+      <c r="H11" s="4"/>
+      <c r="I11" s="4"/>
+      <c r="J11" s="4"/>
+      <c r="K11" s="4"/>
+      <c r="L11" s="4"/>
+      <c r="M11" s="4"/>
+      <c r="N11" s="4"/>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="A12" s="4"/>
+      <c r="B12" s="4"/>
+      <c r="C12" s="4"/>
+      <c r="D12" s="4"/>
+      <c r="E12" s="4"/>
+      <c r="F12" s="4"/>
+      <c r="G12" s="4"/>
+      <c r="H12" s="4"/>
+      <c r="I12" s="4"/>
+      <c r="J12" s="4"/>
+      <c r="K12" s="4"/>
+      <c r="L12" s="4"/>
+      <c r="M12" s="4"/>
+      <c r="N12" s="4"/>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="A13" s="4"/>
+      <c r="B13" s="4"/>
+      <c r="C13" s="4"/>
+      <c r="D13" s="4"/>
+      <c r="E13" s="4"/>
+      <c r="F13" s="4"/>
+      <c r="G13" s="4"/>
+      <c r="H13" s="4"/>
+      <c r="I13" s="4"/>
+      <c r="J13" s="4"/>
+      <c r="K13" s="4"/>
+      <c r="L13" s="4"/>
+      <c r="M13" s="4"/>
+      <c r="N13" s="4"/>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="A14" s="4"/>
+      <c r="B14" s="4"/>
+      <c r="C14" s="4"/>
+      <c r="D14" s="4"/>
+      <c r="E14" s="4"/>
+      <c r="F14" s="4"/>
+      <c r="G14" s="4"/>
+      <c r="H14" s="4"/>
+      <c r="I14" s="4"/>
+      <c r="J14" s="4"/>
+      <c r="K14" s="4"/>
+      <c r="L14" s="4"/>
+      <c r="M14" s="4"/>
+      <c r="N14" s="4"/>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="A15" s="4"/>
+      <c r="B15" s="4"/>
+      <c r="C15" s="4"/>
+      <c r="D15" s="4"/>
+      <c r="E15" s="4"/>
+      <c r="F15" s="4"/>
+      <c r="G15" s="4"/>
+      <c r="H15" s="4"/>
+      <c r="I15" s="4"/>
+      <c r="J15" s="4"/>
+      <c r="K15" s="4"/>
+      <c r="L15" s="4"/>
+      <c r="M15" s="4"/>
+      <c r="N15" s="4"/>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="A16" s="4"/>
+      <c r="B16" s="4"/>
+      <c r="C16" s="4"/>
+      <c r="D16" s="4"/>
+      <c r="E16" s="4"/>
+      <c r="F16" s="4"/>
+      <c r="G16" s="4"/>
+      <c r="H16" s="4"/>
+      <c r="I16" s="4"/>
+      <c r="J16" s="4"/>
+      <c r="K16" s="4"/>
+      <c r="L16" s="4"/>
+      <c r="M16" s="4"/>
+      <c r="N16" s="4"/>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="A17" s="4"/>
+      <c r="B17" s="4"/>
+      <c r="C17" s="4"/>
+      <c r="D17" s="4"/>
+      <c r="E17" s="4"/>
+      <c r="F17" s="4"/>
+      <c r="G17" s="4"/>
+      <c r="H17" s="4"/>
+      <c r="I17" s="4"/>
+      <c r="J17" s="4"/>
+      <c r="K17" s="4"/>
+      <c r="L17" s="4"/>
+      <c r="M17" s="4"/>
+      <c r="N17" s="4"/>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="A18" s="4"/>
+      <c r="B18" s="4"/>
+      <c r="C18" s="4"/>
+      <c r="D18" s="4"/>
+      <c r="E18" s="4"/>
+      <c r="F18" s="4"/>
+      <c r="G18" s="4"/>
+      <c r="H18" s="4"/>
+      <c r="I18" s="4"/>
+      <c r="J18" s="4"/>
+      <c r="K18" s="4"/>
+      <c r="L18" s="4"/>
+      <c r="M18" s="4"/>
+      <c r="N18" s="4"/>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="A19" s="4"/>
+      <c r="B19" s="4"/>
+      <c r="C19" s="4"/>
+      <c r="D19" s="4"/>
+      <c r="E19" s="4"/>
+      <c r="F19" s="4"/>
+      <c r="G19" s="4"/>
+      <c r="H19" s="4"/>
+      <c r="I19" s="4"/>
+      <c r="J19" s="4"/>
+      <c r="K19" s="4"/>
+      <c r="L19" s="4"/>
+      <c r="M19" s="4"/>
+      <c r="N19" s="4"/>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="A20" s="4"/>
+      <c r="B20" s="4"/>
+      <c r="C20" s="4"/>
+      <c r="D20" s="4"/>
+      <c r="E20" s="4"/>
+      <c r="F20" s="4"/>
+      <c r="G20" s="4"/>
+      <c r="H20" s="4"/>
+      <c r="I20" s="4"/>
+      <c r="J20" s="4"/>
+      <c r="K20" s="4"/>
+      <c r="L20" s="4"/>
+      <c r="M20" s="4"/>
+      <c r="N20" s="4"/>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="A21" s="4"/>
+      <c r="B21" s="4"/>
+      <c r="C21" s="4"/>
+      <c r="D21" s="4"/>
+      <c r="E21" s="4"/>
+      <c r="F21" s="4"/>
+      <c r="G21" s="4"/>
+      <c r="H21" s="4"/>
+      <c r="I21" s="4"/>
+      <c r="J21" s="4"/>
+      <c r="K21" s="4"/>
+      <c r="L21" s="4"/>
+      <c r="M21" s="4"/>
+      <c r="N21" s="4"/>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="A22" s="4"/>
+      <c r="B22" s="4"/>
+      <c r="C22" s="4"/>
+      <c r="D22" s="4"/>
+      <c r="E22" s="4"/>
+      <c r="F22" s="4"/>
+      <c r="G22" s="4"/>
+      <c r="H22" s="4"/>
+      <c r="I22" s="4"/>
+      <c r="J22" s="4"/>
+      <c r="K22" s="4"/>
+      <c r="L22" s="4"/>
+      <c r="M22" s="4"/>
+      <c r="N22" s="4"/>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="A23" s="4"/>
+      <c r="B23" s="4"/>
+      <c r="C23" s="4"/>
+      <c r="D23" s="4"/>
+      <c r="E23" s="4"/>
+      <c r="F23" s="4"/>
+      <c r="G23" s="4"/>
+      <c r="H23" s="4"/>
+      <c r="I23" s="4"/>
+      <c r="J23" s="4"/>
+      <c r="K23" s="4"/>
+      <c r="L23" s="4"/>
+      <c r="M23" s="4"/>
+      <c r="N23" s="4"/>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="A24" s="4"/>
+      <c r="B24" s="4"/>
+      <c r="C24" s="4"/>
+      <c r="D24" s="4"/>
+      <c r="E24" s="4"/>
+      <c r="F24" s="4"/>
+      <c r="G24" s="4"/>
+      <c r="H24" s="4"/>
+      <c r="I24" s="4"/>
+      <c r="J24" s="4"/>
+      <c r="K24" s="4"/>
+      <c r="L24" s="4"/>
+      <c r="M24" s="4"/>
+      <c r="N24" s="4"/>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="A25" s="4"/>
+      <c r="B25" s="4"/>
+      <c r="C25" s="4"/>
+      <c r="D25" s="4"/>
+      <c r="E25" s="4"/>
+      <c r="F25" s="4"/>
+      <c r="G25" s="4"/>
+      <c r="H25" s="4"/>
+      <c r="I25" s="4"/>
+      <c r="J25" s="4"/>
+      <c r="K25" s="4"/>
+      <c r="L25" s="4"/>
+      <c r="M25" s="4"/>
+      <c r="N25" s="4"/>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="A26" s="4"/>
+      <c r="B26" s="4"/>
+      <c r="C26" s="4"/>
+      <c r="D26" s="4"/>
+      <c r="E26" s="4"/>
+      <c r="F26" s="4"/>
+      <c r="G26" s="4"/>
+      <c r="H26" s="4"/>
+      <c r="I26" s="4"/>
+      <c r="J26" s="4"/>
+      <c r="K26" s="4"/>
+      <c r="L26" s="4"/>
+      <c r="M26" s="4"/>
+      <c r="N26" s="4"/>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="A27" s="4"/>
+      <c r="B27" s="4"/>
+      <c r="C27" s="4"/>
+      <c r="D27" s="4"/>
+      <c r="E27" s="4"/>
+      <c r="F27" s="4"/>
+      <c r="G27" s="4"/>
+      <c r="H27" s="4"/>
+      <c r="I27" s="4"/>
+      <c r="J27" s="4"/>
+      <c r="K27" s="4"/>
+      <c r="L27" s="4"/>
+      <c r="M27" s="4"/>
+      <c r="N27" s="4"/>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="A28" s="4"/>
+      <c r="B28" s="4"/>
+      <c r="C28" s="4"/>
+      <c r="D28" s="4"/>
+      <c r="E28" s="4"/>
+      <c r="F28" s="4"/>
+      <c r="G28" s="4"/>
+      <c r="H28" s="4"/>
+      <c r="I28" s="4"/>
+      <c r="J28" s="4"/>
+      <c r="K28" s="4"/>
+      <c r="L28" s="4"/>
+      <c r="M28" s="4"/>
+      <c r="N28" s="4"/>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="A29" s="4"/>
+      <c r="B29" s="4"/>
+      <c r="C29" s="4"/>
+      <c r="D29" s="4"/>
+      <c r="E29" s="4"/>
+      <c r="F29" s="4"/>
+      <c r="G29" s="4"/>
+      <c r="H29" s="4"/>
+      <c r="I29" s="4"/>
+      <c r="J29" s="4"/>
+      <c r="K29" s="4"/>
+      <c r="L29" s="4"/>
+      <c r="M29" s="4"/>
+      <c r="N29" s="4"/>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="A30" s="4"/>
+      <c r="B30" s="4"/>
+      <c r="C30" s="4"/>
+      <c r="D30" s="4"/>
+      <c r="E30" s="4"/>
+      <c r="F30" s="4"/>
+      <c r="G30" s="4"/>
+      <c r="H30" s="4"/>
+      <c r="I30" s="4"/>
+      <c r="J30" s="4"/>
+      <c r="K30" s="4"/>
+      <c r="L30" s="4"/>
+      <c r="M30" s="4"/>
+      <c r="N30" s="4"/>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="A31" s="4"/>
+      <c r="B31" s="4"/>
+      <c r="C31" s="4"/>
+      <c r="D31" s="4"/>
+      <c r="E31" s="4"/>
+      <c r="F31" s="4"/>
+      <c r="G31" s="4"/>
+      <c r="H31" s="4"/>
+      <c r="I31" s="4"/>
+      <c r="J31" s="4"/>
+      <c r="K31" s="4"/>
+      <c r="L31" s="4"/>
+      <c r="M31" s="4"/>
+      <c r="N31" s="4"/>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="A32" s="4"/>
+      <c r="B32" s="4"/>
+      <c r="C32" s="4"/>
+      <c r="D32" s="4"/>
+      <c r="E32" s="4"/>
+      <c r="F32" s="4"/>
+      <c r="G32" s="4"/>
+      <c r="H32" s="4"/>
+      <c r="I32" s="4"/>
+      <c r="J32" s="4"/>
+      <c r="K32" s="4"/>
+      <c r="L32" s="4"/>
+      <c r="M32" s="4"/>
+      <c r="N32" s="4"/>
+    </row>
+    <row r="33" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="A33" s="4"/>
+      <c r="B33" s="4"/>
+      <c r="C33" s="4"/>
+      <c r="D33" s="4"/>
+      <c r="E33" s="4"/>
+      <c r="F33" s="4"/>
+      <c r="G33" s="4"/>
+      <c r="H33" s="4"/>
+      <c r="I33" s="4"/>
+      <c r="J33" s="4"/>
+      <c r="K33" s="4"/>
+      <c r="L33" s="4"/>
+      <c r="M33" s="4"/>
+      <c r="N33" s="4"/>
+    </row>
+    <row r="34" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="A34" s="4"/>
+      <c r="B34" s="4"/>
+      <c r="C34" s="4"/>
+      <c r="D34" s="4"/>
+      <c r="E34" s="4"/>
+      <c r="F34" s="4"/>
+      <c r="G34" s="4"/>
+      <c r="H34" s="4"/>
+      <c r="I34" s="4"/>
+      <c r="J34" s="4"/>
+      <c r="K34" s="4"/>
+      <c r="L34" s="4"/>
+      <c r="M34" s="4"/>
+      <c r="N34" s="4"/>
+    </row>
+    <row r="35" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="A35" s="4"/>
+      <c r="B35" s="4"/>
+      <c r="C35" s="4"/>
+      <c r="D35" s="4"/>
+      <c r="E35" s="4"/>
+      <c r="F35" s="4"/>
+      <c r="G35" s="4"/>
+      <c r="H35" s="4"/>
+      <c r="I35" s="4"/>
+      <c r="J35" s="4"/>
+      <c r="K35" s="4"/>
+      <c r="L35" s="4"/>
+      <c r="M35" s="4"/>
+      <c r="N35" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -781,57 +1226,55 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
   <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="34.86328125" customWidth="1"/>
     <col min="2" max="2" width="23.73046875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="B1" s="7" t="s">
-        <v>37</v>
+      <c r="B1" s="5" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B2" s="5">
-        <f>SUM(Data!B3,Data!B7)/SUM(Data!B3,Data!B7,Data!B11,Data!B15)</f>
-        <v>0.42384105960264901</v>
+        <v>2</v>
+      </c>
+      <c r="B2" s="4">
+        <f>Data!B2</f>
+        <v>0.501</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
-        <v>22</v>
-      </c>
-      <c r="B3" s="5">
-        <f>SUM(Data!B11,Data!B16,Data!B18/2)/SUM(Data!B3,Data!B7,Data!B11,Data!B15)</f>
-        <v>0.52814569536423839</v>
+        <v>5</v>
+      </c>
+      <c r="B3" s="4">
+        <f>Data!B5</f>
+        <v>6.9860000000000033E-2</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
-        <v>23</v>
-      </c>
-      <c r="B4" s="5">
-        <f>(Data!B18/2)/SUM(Data!B3,Data!B7,Data!B11,Data!B15)</f>
-        <v>4.8013245033112585E-2</v>
+        <v>6</v>
+      </c>
+      <c r="B4" s="4">
+        <f>Data!B4</f>
+        <v>0.42913999999999997</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
-        <v>21</v>
+        <v>4</v>
       </c>
       <c r="B5">
         <v>0</v>
@@ -839,7 +1282,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
-        <v>24</v>
+        <v>7</v>
       </c>
       <c r="B6">
         <v>0</v>
@@ -847,7 +1290,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
-        <v>25</v>
+        <v>8</v>
       </c>
       <c r="B7">
         <v>0</v>
@@ -855,7 +1298,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
-        <v>26</v>
+        <v>9</v>
       </c>
       <c r="B8">
         <v>0</v>
@@ -863,7 +1306,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
-        <v>27</v>
+        <v>10</v>
       </c>
       <c r="B9">
         <v>0</v>
@@ -871,7 +1314,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
-        <v>28</v>
+        <v>11</v>
       </c>
       <c r="B10">
         <v>0</v>

</xml_diff>